<commit_message>
DC Finanzas y ActualizacionCronograma
</commit_message>
<xml_diff>
--- a/cronograma de actividades.xlsx
+++ b/cronograma de actividades.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani\Desktop\PROYECTOPARCIAL1\ProyectoParcial1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Desktop\UMG\PROGRA3\ProyectoParcial1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC490DF-05E4-47B2-9413-8541FDAA18C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -137,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,6 +342,48 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -347,48 +398,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -670,11 +679,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18:N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,30 +693,30 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="5" spans="3:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="3:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
@@ -716,24 +725,24 @@
       <c r="D6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27" t="s">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27" t="s">
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="8">
@@ -742,24 +751,24 @@
       <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="23">
         <v>43867</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22">
+      <c r="F7" s="23"/>
+      <c r="G7" s="23">
         <v>43867</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="19" t="s">
+      <c r="H7" s="24"/>
+      <c r="I7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="30">
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="15">
         <v>1</v>
       </c>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="8">
@@ -769,24 +778,24 @@
       <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="25">
         <v>43867</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="17">
+      <c r="F8" s="22"/>
+      <c r="G8" s="25">
         <v>43870</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20">
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="18">
         <v>1</v>
       </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" s="8">
@@ -795,24 +804,24 @@
       <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="25">
         <v>43867</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="17">
+      <c r="F9" s="22"/>
+      <c r="G9" s="25">
         <v>43868</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19" t="s">
+      <c r="H9" s="22"/>
+      <c r="I9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20">
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="18">
         <v>1</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="8">
@@ -821,24 +830,24 @@
       <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="25">
         <v>43867</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="17">
+      <c r="F10" s="22"/>
+      <c r="G10" s="25">
         <v>43867</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="19" t="s">
+      <c r="H10" s="22"/>
+      <c r="I10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20">
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="18">
         <v>1</v>
       </c>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
     </row>
     <row r="11" spans="3:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="8">
@@ -847,16 +856,16 @@
       <c r="D11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="8">
@@ -865,82 +874,82 @@
       <c r="D12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="25">
         <v>43867</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="17">
+      <c r="F13" s="22"/>
+      <c r="G13" s="25">
         <v>43871</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19" t="s">
+      <c r="H13" s="22"/>
+      <c r="I13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C14" s="8"/>
       <c r="D14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="25">
         <v>43867</v>
       </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="17">
+      <c r="F14" s="22"/>
+      <c r="G14" s="25">
         <v>43871</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="19" t="s">
+      <c r="H14" s="22"/>
+      <c r="I14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C15" s="8"/>
       <c r="D15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="25">
         <v>43868</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="17">
+      <c r="F15" s="22"/>
+      <c r="G15" s="25">
         <v>43875</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19" t="s">
+      <c r="H15" s="22"/>
+      <c r="I15" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="8">
@@ -949,82 +958,84 @@
       <c r="D16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="8"/>
       <c r="D17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="25">
         <v>43867</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="17">
+      <c r="F17" s="22"/>
+      <c r="G17" s="25">
         <v>43871</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="19" t="s">
+      <c r="H17" s="22"/>
+      <c r="I17" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="18">
+        <v>1</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="8"/>
       <c r="D18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="25">
         <v>43867</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="17">
+      <c r="F18" s="22"/>
+      <c r="G18" s="25">
         <v>43871</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="19" t="s">
+      <c r="H18" s="22"/>
+      <c r="I18" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" s="8"/>
       <c r="D19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="25">
         <v>43868</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="17">
+      <c r="F19" s="22"/>
+      <c r="G19" s="25">
         <v>43875</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="8">
@@ -1033,82 +1044,82 @@
       <c r="D20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" s="8"/>
       <c r="D21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="25">
         <v>43867</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="17">
+      <c r="F21" s="22"/>
+      <c r="G21" s="25">
         <v>43871</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="19" t="s">
+      <c r="H21" s="22"/>
+      <c r="I21" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="25">
         <v>43867</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="17">
+      <c r="F22" s="22"/>
+      <c r="G22" s="25">
         <v>43871</v>
       </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="19" t="s">
+      <c r="H22" s="22"/>
+      <c r="I22" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" s="8"/>
       <c r="D23" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="25">
         <v>43868</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="17">
+      <c r="F23" s="22"/>
+      <c r="G23" s="25">
         <v>43875</v>
       </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="19" t="s">
+      <c r="H23" s="22"/>
+      <c r="I23" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" s="8">
@@ -1117,204 +1128,204 @@
       <c r="D24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="D25" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" s="8"/>
       <c r="D26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" s="8"/>
       <c r="D27" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="21"/>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="21"/>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C30" s="8"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C31" s="8"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C35" s="8"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C38" s="8">
@@ -1323,16 +1334,16 @@
       <c r="D38" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C39" s="8">
@@ -1341,16 +1352,16 @@
       <c r="D39" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
     </row>
     <row r="40" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C40" s="8">
@@ -1359,80 +1370,80 @@
       <c r="D40" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="17"/>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C41" s="8"/>
       <c r="D41" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C42" s="8"/>
       <c r="D42" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
     </row>
     <row r="43" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C43" s="8"/>
       <c r="D43" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="21"/>
-      <c r="N43" s="21"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
     </row>
     <row r="44" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C44" s="8"/>
       <c r="D44" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
-      <c r="N44" s="21"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
     </row>
     <row r="45" spans="3:14" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
@@ -1449,61 +1460,69 @@
     </row>
   </sheetData>
   <mergeCells count="160">
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="L33:N33"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="L24:N24"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
@@ -1528,60 +1547,67 @@
     <mergeCell ref="L37:N37"/>
     <mergeCell ref="L38:N38"/>
     <mergeCell ref="L39:N39"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="L12:N12"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="L29:N29"/>
     <mergeCell ref="L15:N15"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
     <mergeCell ref="L10:N10"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
     <mergeCell ref="L9:N9"/>
-    <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="E24:F24"/>
@@ -1594,21 +1620,6 @@
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>